<commit_message>
Cambios pre entrega TFM
Generar grafico de evolucion 2018-2023 de todas las empresas. Introducir nuevo método para el calculo del tamaño de los nodos en el grafo
</commit_message>
<xml_diff>
--- a/data/tickers.xlsx
+++ b/data/tickers.xlsx
@@ -10,8 +10,8 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7miWCISrNrP7lODQBq6ch5f34hYK/g=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="FWE5ESgulOG74LPHpZtuTtsa/mD9yUV9Iavtr2is6Rw="/>
     </ext>
   </extLst>
 </workbook>
@@ -426,12 +426,12 @@
     </font>
     <font>
       <color rgb="FF717171"/>
-      <name val="Open-sans"/>
+      <name val="Open Sans"/>
     </font>
     <font>
       <sz val="9.0"/>
       <color rgb="FF232A31"/>
-      <name val="&quot;Yahoo Sans Finance&quot;"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -454,26 +454,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -721,10 +711,10 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -732,692 +722,692 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5"/>
+      <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5"/>
+      <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="5"/>
+      <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="5"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D23" s="5"/>
+      <c r="D23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="5"/>
+      <c r="D24" s="2"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="5"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="5"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="5"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="5"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="5"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="5"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="5"/>
+      <c r="D39" s="2"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="5"/>
+      <c r="D40" s="2"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="5"/>
+      <c r="D41" s="2"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="5"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D43" s="5"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D44" s="5"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="5"/>
+      <c r="D45" s="2"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="5"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="5"/>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D48" s="5"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="5"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="5"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D51" s="5"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D52" s="5"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="5"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="5"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D55" s="5"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D56" s="5"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="5"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D58" s="5"/>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="8"/>
+      <c r="A59" s="4"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="5"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7"/>
+      <c r="A60" s="4"/>
+      <c r="B60" s="4"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="9"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="10"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" ht="15.75" customHeight="1"/>
     <row r="65" ht="15.75" customHeight="1"/>

</xml_diff>